<commit_message>
multithread counter done. It can create 2 threads, one for even numbers and one for odd numbers
</commit_message>
<xml_diff>
--- a/Modulos/PSP/Tema_1/Teoría Tema1 Algoritmos 2.xlsx
+++ b/Modulos/PSP/Tema_1/Teoría Tema1 Algoritmos 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josemurciabelmonte/Documents/DAM/SEGUNDO CURSO/DAMSecondYear/Modulos/PSP/Tema_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C908FC-85C1-7E46-AC1B-31A74FA17B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E370029-CDCB-CA4A-B317-64DD13B14C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="820" windowWidth="26940" windowHeight="18820" xr2:uid="{B0C67053-691C-EC4F-81B0-39C036F60149}"/>
+    <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="18820" xr2:uid="{B0C67053-691C-EC4F-81B0-39C036F60149}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,10 +92,10 @@
     <t>Quantum</t>
   </si>
   <si>
-    <t>Ante igualdad de tiempo de llegada, ejecuto primero el que antes estuviese</t>
+    <t>TIEMPO</t>
   </si>
   <si>
-    <t>TIEMPO</t>
+    <t>Ante igualdad de tiempo de llegada, ejecuto primero el que dura menos</t>
   </si>
 </sst>
 </file>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E19AE84-7FE4-BB42-800D-37CC1FDAEDBA}">
   <dimension ref="A2:BB88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,7 +1059,7 @@
         <v>20</v>
       </c>
       <c r="AD17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AJ17">
         <v>29</v>
@@ -1441,7 +1441,7 @@
         <v>20</v>
       </c>
       <c r="AD39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AJ39">
         <v>29</v>
@@ -1654,9 +1654,8 @@
         <v>4</v>
       </c>
       <c r="I53" s="17"/>
-      <c r="M53" s="12"/>
+      <c r="M53" s="35"/>
       <c r="N53" s="12"/>
-      <c r="O53" s="35"/>
     </row>
     <row r="54" spans="2:40" x14ac:dyDescent="0.2">
       <c r="H54" s="19"/>
@@ -1675,8 +1674,9 @@
       </c>
       <c r="I55" s="17"/>
       <c r="L55" s="32"/>
-      <c r="M55" s="32"/>
+      <c r="M55" s="12"/>
       <c r="N55" s="32"/>
+      <c r="O55" s="32"/>
     </row>
     <row r="56" spans="2:40" x14ac:dyDescent="0.2">
       <c r="D56" s="11" t="s">
@@ -1820,7 +1820,7 @@
         <v>20</v>
       </c>
       <c r="AD61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AJ61">
         <v>29</v>
@@ -1920,17 +1920,17 @@
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
       <c r="N71" s="18"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="36"/>
+      <c r="O71" s="34"/>
+      <c r="P71" s="12"/>
       <c r="Q71" s="12"/>
       <c r="R71" s="12"/>
-      <c r="S71" s="12"/>
+      <c r="S71" s="36"/>
       <c r="T71" s="12"/>
-      <c r="U71" s="36"/>
+      <c r="U71" s="12"/>
       <c r="V71" s="12"/>
-      <c r="W71" s="12"/>
+      <c r="W71" s="36"/>
       <c r="X71" s="12"/>
-      <c r="Y71" s="36"/>
+      <c r="Y71" s="12"/>
       <c r="Z71" s="12"/>
       <c r="AA71" s="36"/>
     </row>
@@ -1973,19 +1973,22 @@
         <v>5</v>
       </c>
       <c r="I73" s="30"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="12"/>
-      <c r="L73" s="8"/>
+      <c r="J73" s="12"/>
+      <c r="K73" s="8"/>
+      <c r="L73" s="12"/>
       <c r="M73" s="12"/>
       <c r="N73" s="18"/>
       <c r="O73" s="12"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="8"/>
+      <c r="P73" s="8"/>
+      <c r="Q73" s="12"/>
       <c r="R73" s="12"/>
       <c r="S73" s="12"/>
       <c r="T73" s="12"/>
-      <c r="U73" s="12"/>
-      <c r="V73" s="8"/>
+      <c r="U73" s="8"/>
+      <c r="V73" s="12"/>
+      <c r="W73" s="12"/>
+      <c r="X73" s="12"/>
+      <c r="Y73" s="8"/>
     </row>
     <row r="74" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B74" s="8" t="s">
@@ -2030,8 +2033,7 @@
       <c r="N75" s="18"/>
       <c r="O75" s="12"/>
       <c r="P75" s="12"/>
-      <c r="Q75" s="12"/>
-      <c r="R75" s="7"/>
+      <c r="Q75" s="7"/>
     </row>
     <row r="76" spans="1:40" x14ac:dyDescent="0.2">
       <c r="H76" s="19"/>
@@ -2051,8 +2053,8 @@
       <c r="I77" s="17"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
-      <c r="O77" s="16"/>
+      <c r="N77" s="16"/>
+      <c r="O77" s="12"/>
       <c r="P77" s="12"/>
       <c r="Q77" s="12"/>
       <c r="R77" s="12"/>
@@ -2068,8 +2070,7 @@
         <v>11</v>
       </c>
       <c r="E78" s="11">
-        <f>SUM(F70:F75)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H78" s="19"/>
       <c r="I78" s="17"/>
@@ -2079,11 +2080,9 @@
         <v>2</v>
       </c>
       <c r="I79" s="17"/>
-      <c r="J79" s="12"/>
-      <c r="K79" s="28"/>
-      <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="5"/>
+      <c r="J79" s="28"/>
+      <c r="K79" s="12"/>
+      <c r="L79" s="5"/>
     </row>
     <row r="80" spans="1:40" x14ac:dyDescent="0.2">
       <c r="D80" s="11" t="s">
@@ -2107,12 +2106,12 @@
       <c r="O81" s="12"/>
       <c r="P81" s="12"/>
       <c r="Q81" s="12"/>
-      <c r="R81" s="12"/>
-      <c r="S81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="12"/>
       <c r="T81" s="12"/>
       <c r="U81" s="12"/>
-      <c r="V81" s="12"/>
-      <c r="W81" s="3"/>
+      <c r="V81" s="3"/>
+      <c r="W81" s="12"/>
       <c r="X81" s="12"/>
       <c r="Y81" s="12"/>
       <c r="Z81" s="37"/>
@@ -2217,7 +2216,7 @@
         <v>20</v>
       </c>
       <c r="AD83" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AJ83">
         <v>29</v>
@@ -2228,7 +2227,7 @@
     </row>
     <row r="88" spans="4:40" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>